<commit_message>
changes not needed, still commiting
</commit_message>
<xml_diff>
--- a/src/main/java/com/adactinhotel/qa/testdata/adactinhotelTestData.xlsx
+++ b/src/main/java/com/adactinhotel/qa/testdata/adactinhotelTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\AdactinHotelApp-master\AdactinHotelApp-master\src\main\java\com\adactinhotel\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\eclipse-workspace\AdactinHotelwebsite\src\main\java\com\adactinhotel\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>cvv</t>
+  </si>
+  <si>
+    <t>CheckinDate</t>
+  </si>
+  <si>
+    <t>CheckoutDate</t>
   </si>
   <si>
     <t>Revathi M</t>
@@ -86,9 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +401,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -403,6 +411,8 @@
     <col min="3" max="3" width="16.57031" customWidth="1"/>
     <col min="4" max="4" width="18.85547" customWidth="1"/>
     <col min="5" max="5" width="11.71094" customWidth="1"/>
+    <col min="6" max="6" width="13.85547" customWidth="1"/>
+    <col min="7" max="7" width="14.28516" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -421,33 +431,45 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>1234567890123460</v>
       </c>
       <c r="E2">
         <v>123</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45628</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45537</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3">
         <v>1234567890123460</v>

</xml_diff>